<commit_message>
Train drift, steer and acceleration together
</commit_message>
<xml_diff>
--- a/evaluate.xlsx
+++ b/evaluate.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,6 +477,8 @@
       <c r="I1" s="1" t="n"/>
       <c r="J1" s="1" t="n"/>
       <c r="K1" s="1" t="n"/>
+      <c r="L1" s="1" t="n"/>
+      <c r="M1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr"/>
@@ -487,45 +489,55 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
+          <t>cum_reward_median</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
           <t>cum_reward_std</t>
         </is>
       </c>
-      <c r="D2" s="1" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
         <is>
           <t>cum_reward_max</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>cum_reward_min</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="G2" s="1" t="inlineStr">
         <is>
           <t>cum_reward_dif</t>
         </is>
       </c>
-      <c r="G2" s="1" t="inlineStr">
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t>steps_mean</t>
         </is>
       </c>
-      <c r="H2" s="1" t="inlineStr">
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>steps_median</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
         <is>
           <t>steps_std</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
+      <c r="K2" s="1" t="inlineStr">
         <is>
           <t>steps_max</t>
         </is>
       </c>
-      <c r="J2" s="1" t="inlineStr">
+      <c r="L2" s="1" t="inlineStr">
         <is>
           <t>steps_min</t>
         </is>
       </c>
-      <c r="K2" s="1" t="inlineStr">
+      <c r="M2" s="1" t="inlineStr">
         <is>
           <t>steps_dif</t>
         </is>
@@ -538,34 +550,40 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>242.83</v>
+        <v>241.29</v>
       </c>
       <c r="C4" t="n">
-        <v>16.9</v>
+        <v>235.69</v>
       </c>
       <c r="D4" t="n">
+        <v>18.8</v>
+      </c>
+      <c r="E4" t="n">
         <v>277.69</v>
       </c>
-      <c r="E4" t="n">
-        <v>222.59</v>
-      </c>
       <c r="F4" t="n">
-        <v>55.1</v>
+        <v>202.61</v>
       </c>
       <c r="G4" t="n">
-        <v>635.9</v>
+        <v>75.08</v>
       </c>
       <c r="H4" t="n">
-        <v>16.83</v>
+        <v>637.45</v>
       </c>
       <c r="I4" t="n">
-        <v>656</v>
+        <v>643</v>
       </c>
       <c r="J4" t="n">
+        <v>18.74</v>
+      </c>
+      <c r="K4" t="n">
+        <v>676</v>
+      </c>
+      <c r="L4" t="n">
         <v>601</v>
       </c>
-      <c r="K4" t="n">
-        <v>55</v>
+      <c r="M4" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="5">
@@ -575,34 +593,40 @@
         </is>
       </c>
       <c r="B5" t="n">
+        <v>429.27</v>
+      </c>
+      <c r="C5" t="n">
         <v>430.08</v>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
       <c r="D5" t="n">
-        <v>430.08</v>
+        <v>3.51</v>
       </c>
       <c r="E5" t="n">
         <v>430.08</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>413.96</v>
       </c>
       <c r="G5" t="n">
-        <v>450</v>
+        <v>16.12</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>450.75</v>
       </c>
       <c r="I5" t="n">
         <v>450</v>
       </c>
       <c r="J5" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="K5" t="n">
+        <v>465</v>
+      </c>
+      <c r="L5" t="n">
         <v>450</v>
       </c>
-      <c r="K5" t="n">
-        <v>0</v>
+      <c r="M5" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="6">
@@ -615,295 +639,515 @@
         <v>465.63</v>
       </c>
       <c r="C6" t="n">
+        <v>465.63</v>
+      </c>
+      <c r="D6" t="n">
         <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>465.63</v>
       </c>
       <c r="E6" t="n">
         <v>465.63</v>
       </c>
       <c r="F6" t="n">
+        <v>465.63</v>
+      </c>
+      <c r="G6" t="n">
         <v>0</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>413</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
       </c>
       <c r="I6" t="n">
         <v>413</v>
       </c>
       <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
         <v>413</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
+        <v>413</v>
+      </c>
+      <c r="M6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>baseline</t>
+          <t>baseline_noDrift</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>273.48</v>
+        <v>211.86</v>
       </c>
       <c r="C7" t="n">
-        <v>20.44</v>
+        <v>219.83</v>
       </c>
       <c r="D7" t="n">
-        <v>303.39</v>
+        <v>16.32</v>
       </c>
       <c r="E7" t="n">
-        <v>229.28</v>
+        <v>229.53</v>
       </c>
       <c r="F7" t="n">
-        <v>74.09999999999999</v>
+        <v>180.43</v>
       </c>
       <c r="G7" t="n">
-        <v>605.3</v>
+        <v>49.11</v>
       </c>
       <c r="H7" t="n">
-        <v>20.45</v>
+        <v>667.05</v>
       </c>
       <c r="I7" t="n">
+        <v>659</v>
+      </c>
+      <c r="J7" t="n">
+        <v>16.15</v>
+      </c>
+      <c r="K7" t="n">
+        <v>698</v>
+      </c>
+      <c r="L7" t="n">
         <v>649</v>
       </c>
-      <c r="J7" t="n">
-        <v>575</v>
-      </c>
-      <c r="K7" t="n">
-        <v>74</v>
+      <c r="M7" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>trans_no_drift_decTransColor1_80</t>
+          <t>baseline</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>199.74</v>
+        <v>276.73</v>
       </c>
       <c r="C8" t="n">
-        <v>18.03</v>
+        <v>280.76</v>
       </c>
       <c r="D8" t="n">
-        <v>224.59</v>
+        <v>21.82</v>
       </c>
       <c r="E8" t="n">
-        <v>180.45</v>
+        <v>305.47</v>
       </c>
       <c r="F8" t="n">
-        <v>44.13</v>
+        <v>228.15</v>
       </c>
       <c r="G8" t="n">
-        <v>679.1</v>
+        <v>77.31999999999999</v>
       </c>
       <c r="H8" t="n">
-        <v>18.22</v>
+        <v>602</v>
       </c>
       <c r="I8" t="n">
-        <v>699</v>
+        <v>598</v>
       </c>
       <c r="J8" t="n">
-        <v>654</v>
+        <v>21.92</v>
       </c>
       <c r="K8" t="n">
-        <v>45</v>
+        <v>651</v>
+      </c>
+      <c r="L8" t="n">
+        <v>573</v>
+      </c>
+      <c r="M8" t="n">
+        <v>78</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>trans_no_drift_decTransColor1_best</t>
+          <t>trans_no_drift_decTransColor1_80</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>187.65</v>
+        <v>202.58</v>
       </c>
       <c r="C9" t="n">
-        <v>12.73</v>
+        <v>197.93</v>
       </c>
       <c r="D9" t="n">
-        <v>219.53</v>
+        <v>18.5</v>
       </c>
       <c r="E9" t="n">
-        <v>173.78</v>
+        <v>226.27</v>
       </c>
       <c r="F9" t="n">
-        <v>45.75</v>
+        <v>178.52</v>
       </c>
       <c r="G9" t="n">
-        <v>691.1</v>
+        <v>47.75</v>
       </c>
       <c r="H9" t="n">
-        <v>12.6</v>
+        <v>676.15</v>
       </c>
       <c r="I9" t="n">
-        <v>705</v>
+        <v>681</v>
       </c>
       <c r="J9" t="n">
-        <v>660</v>
+        <v>18.52</v>
       </c>
       <c r="K9" t="n">
-        <v>45</v>
+        <v>700</v>
+      </c>
+      <c r="L9" t="n">
+        <v>653</v>
+      </c>
+      <c r="M9" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>trans_drift_0</t>
+          <t>trans_no_drift_decTransColor1_best</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>288.54</v>
+        <v>188.93</v>
       </c>
       <c r="C10" t="n">
-        <v>5.83</v>
+        <v>178.88</v>
       </c>
       <c r="D10" t="n">
-        <v>293.42</v>
+        <v>17.87</v>
       </c>
       <c r="E10" t="n">
-        <v>272.29</v>
+        <v>225.25</v>
       </c>
       <c r="F10" t="n">
-        <v>21.13</v>
+        <v>175.27</v>
       </c>
       <c r="G10" t="n">
-        <v>590.2</v>
+        <v>49.98</v>
       </c>
       <c r="H10" t="n">
-        <v>6.01</v>
+        <v>689.9</v>
       </c>
       <c r="I10" t="n">
-        <v>607</v>
+        <v>700</v>
       </c>
       <c r="J10" t="n">
-        <v>585</v>
+        <v>17.84</v>
       </c>
       <c r="K10" t="n">
-        <v>22</v>
+        <v>703</v>
+      </c>
+      <c r="L10" t="n">
+        <v>653</v>
+      </c>
+      <c r="M10" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>trans_drift_1</t>
+          <t>trans_drift_0</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>264.83</v>
+        <v>286.23</v>
       </c>
       <c r="C11" t="n">
-        <v>27.16</v>
+        <v>288.94</v>
       </c>
       <c r="D11" t="n">
-        <v>302.74</v>
+        <v>7.81</v>
       </c>
       <c r="E11" t="n">
-        <v>219.06</v>
+        <v>296.4</v>
       </c>
       <c r="F11" t="n">
-        <v>83.68000000000001</v>
+        <v>263.72</v>
       </c>
       <c r="G11" t="n">
-        <v>614.4</v>
+        <v>32.68</v>
       </c>
       <c r="H11" t="n">
-        <v>27.3</v>
+        <v>592.75</v>
       </c>
       <c r="I11" t="n">
-        <v>660</v>
+        <v>590.5</v>
       </c>
       <c r="J11" t="n">
-        <v>576</v>
+        <v>7.62</v>
       </c>
       <c r="K11" t="n">
-        <v>84</v>
+        <v>615</v>
+      </c>
+      <c r="L11" t="n">
+        <v>583</v>
+      </c>
+      <c r="M11" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>trans_drift_2</t>
+          <t>trans_drift_1</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>286.64</v>
+        <v>287.35</v>
       </c>
       <c r="C12" t="n">
-        <v>8.710000000000001</v>
+        <v>288.26</v>
       </c>
       <c r="D12" t="n">
-        <v>302.89</v>
+        <v>6.95</v>
       </c>
       <c r="E12" t="n">
-        <v>273.1</v>
+        <v>299.8</v>
       </c>
       <c r="F12" t="n">
-        <v>29.79</v>
+        <v>275.13</v>
       </c>
       <c r="G12" t="n">
-        <v>592.5</v>
+        <v>24.67</v>
       </c>
       <c r="H12" t="n">
-        <v>8.58</v>
+        <v>591.55</v>
       </c>
       <c r="I12" t="n">
-        <v>605</v>
+        <v>591</v>
       </c>
       <c r="J12" t="n">
-        <v>577</v>
+        <v>6.82</v>
       </c>
       <c r="K12" t="n">
-        <v>28</v>
+        <v>603</v>
+      </c>
+      <c r="L12" t="n">
+        <v>579</v>
+      </c>
+      <c r="M12" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
+          <t>trans_drift_2</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>276.25</v>
+      </c>
+      <c r="C13" t="n">
+        <v>276.17</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="E13" t="n">
+        <v>282.62</v>
+      </c>
+      <c r="F13" t="n">
+        <v>266.48</v>
+      </c>
+      <c r="G13" t="n">
+        <v>16.14</v>
+      </c>
+      <c r="H13" t="n">
+        <v>602.55</v>
+      </c>
+      <c r="I13" t="n">
+        <v>602.5</v>
+      </c>
+      <c r="J13" t="n">
+        <v>4.07</v>
+      </c>
+      <c r="K13" t="n">
+        <v>613</v>
+      </c>
+      <c r="L13" t="n">
+        <v>597</v>
+      </c>
+      <c r="M13" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
           <t>trans_drift_3</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>277.95</v>
-      </c>
-      <c r="C13" t="n">
-        <v>4.37</v>
-      </c>
-      <c r="D13" t="n">
-        <v>283.48</v>
-      </c>
-      <c r="E13" t="n">
-        <v>270.3</v>
-      </c>
-      <c r="F13" t="n">
-        <v>13.18</v>
-      </c>
-      <c r="G13" t="n">
-        <v>600.9</v>
-      </c>
-      <c r="H13" t="n">
-        <v>4.23</v>
-      </c>
-      <c r="I13" t="n">
-        <v>608</v>
-      </c>
-      <c r="J13" t="n">
-        <v>595</v>
-      </c>
-      <c r="K13" t="n">
-        <v>13</v>
+      <c r="B14" t="n">
+        <v>270.93</v>
+      </c>
+      <c r="C14" t="n">
+        <v>267.54</v>
+      </c>
+      <c r="D14" t="n">
+        <v>19.22</v>
+      </c>
+      <c r="E14" t="n">
+        <v>305.33</v>
+      </c>
+      <c r="F14" t="n">
+        <v>234.92</v>
+      </c>
+      <c r="G14" t="n">
+        <v>70.41</v>
+      </c>
+      <c r="H14" t="n">
+        <v>608.05</v>
+      </c>
+      <c r="I14" t="n">
+        <v>611.5</v>
+      </c>
+      <c r="J14" t="n">
+        <v>19.19</v>
+      </c>
+      <c r="K14" t="n">
+        <v>644</v>
+      </c>
+      <c r="L14" t="n">
+        <v>573</v>
+      </c>
+      <c r="M14" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>trans_drift_acc_0</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>266.47</v>
+      </c>
+      <c r="C15" t="n">
+        <v>272.34</v>
+      </c>
+      <c r="D15" t="n">
+        <v>32.07</v>
+      </c>
+      <c r="E15" t="n">
+        <v>317.17</v>
+      </c>
+      <c r="F15" t="n">
+        <v>198.43</v>
+      </c>
+      <c r="G15" t="n">
+        <v>118.74</v>
+      </c>
+      <c r="H15" t="n">
+        <v>612.25</v>
+      </c>
+      <c r="I15" t="n">
+        <v>606</v>
+      </c>
+      <c r="J15" t="n">
+        <v>32.19</v>
+      </c>
+      <c r="K15" t="n">
+        <v>681</v>
+      </c>
+      <c r="L15" t="n">
+        <v>561</v>
+      </c>
+      <c r="M15" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>trans_drift_acc_1</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>281.08</v>
+      </c>
+      <c r="C16" t="n">
+        <v>290.17</v>
+      </c>
+      <c r="D16" t="n">
+        <v>28.61</v>
+      </c>
+      <c r="E16" t="n">
+        <v>317.78</v>
+      </c>
+      <c r="F16" t="n">
+        <v>212.4</v>
+      </c>
+      <c r="G16" t="n">
+        <v>105.38</v>
+      </c>
+      <c r="H16" t="n">
+        <v>597.95</v>
+      </c>
+      <c r="I16" t="n">
+        <v>588.5</v>
+      </c>
+      <c r="J16" t="n">
+        <v>28.78</v>
+      </c>
+      <c r="K16" t="n">
+        <v>667</v>
+      </c>
+      <c r="L16" t="n">
+        <v>561</v>
+      </c>
+      <c r="M16" t="n">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>trans_drift_acc_2</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>266.65</v>
+      </c>
+      <c r="C17" t="n">
+        <v>262.31</v>
+      </c>
+      <c r="D17" t="n">
+        <v>29.51</v>
+      </c>
+      <c r="E17" t="n">
+        <v>314.4</v>
+      </c>
+      <c r="F17" t="n">
+        <v>212.58</v>
+      </c>
+      <c r="G17" t="n">
+        <v>101.83</v>
+      </c>
+      <c r="H17" t="n">
+        <v>612.2</v>
+      </c>
+      <c r="I17" t="n">
+        <v>616.5</v>
+      </c>
+      <c r="J17" t="n">
+        <v>29.46</v>
+      </c>
+      <c r="K17" t="n">
+        <v>666</v>
+      </c>
+      <c r="L17" t="n">
+        <v>565</v>
+      </c>
+      <c r="M17" t="n">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B1:M1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>